<commit_message>
Liste commande Traduit Zied
</commit_message>
<xml_diff>
--- a/docs/Traducteur.xlsx
+++ b/docs/Traducteur.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Developpement\DWWM-RZied\Rjeb Zied\PHPWeb\VirtualhostZied\Projet Pharmacie\Pharmacie\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E42C1B-07F7-4163-A4CF-D14CC973A311}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDADF98F-CD70-4825-8573-8F89CEF77CF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="95">
   <si>
     <t>Header</t>
   </si>
@@ -289,6 +289,27 @@
   </si>
   <si>
     <t>Register</t>
+  </si>
+  <si>
+    <t>ListeCommandes</t>
+  </si>
+  <si>
+    <t>Ajouter une Commande</t>
+  </si>
+  <si>
+    <t>Add an Order</t>
+  </si>
+  <si>
+    <t>Date de Commande</t>
+  </si>
+  <si>
+    <t>Date de reception</t>
+  </si>
+  <si>
+    <t>Date of Order</t>
+  </si>
+  <si>
+    <t>Reception Date</t>
   </si>
 </sst>
 </file>
@@ -638,10 +659,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F44" workbookViewId="0">
-      <selection activeCell="J65" sqref="J65:J66"/>
+    <sheetView tabSelected="1" topLeftCell="G57" workbookViewId="0">
+      <selection activeCell="I71" sqref="I71:I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,7 +673,7 @@
     <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.42578125" customWidth="1"/>
     <col min="9" max="9" width="122.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="95.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="115.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -979,7 +1000,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>46</v>
       </c>
@@ -987,7 +1008,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>47</v>
       </c>
@@ -995,7 +1016,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>48</v>
       </c>
@@ -1003,7 +1024,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>49</v>
       </c>
@@ -1011,7 +1032,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>50</v>
       </c>
@@ -1019,7 +1040,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>51</v>
       </c>
@@ -1027,7 +1048,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>52</v>
       </c>
@@ -1035,47 +1056,95 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
       <c r="D42" t="s">
         <v>55</v>
       </c>
+      <c r="E42" t="s">
+        <v>5</v>
+      </c>
       <c r="F42" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I42" t="str">
+        <f>"INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"""&amp;D42&amp;""","""&amp;C42&amp;""","""&amp;D42&amp;""");"</f>
+        <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Ajouter un Lieu","FR","Ajouter un Lieu");</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" ref="J42:J45" si="0">"INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"""&amp;D42&amp;""","""&amp;E42&amp;""","""&amp;F42&amp;""");"</f>
+        <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Ajouter un Lieu","EN","Add a Place");</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
       <c r="D43" t="s">
         <v>41</v>
       </c>
+      <c r="E43" t="s">
+        <v>5</v>
+      </c>
       <c r="F43" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I43" t="str">
+        <f t="shared" ref="I43:I46" si="1">"INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"""&amp;D43&amp;""","""&amp;C43&amp;""","""&amp;D43&amp;""");"</f>
+        <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Details","FR","Details");</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Details","EN","Details");</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
       <c r="D44" t="s">
         <v>42</v>
       </c>
+      <c r="E44" t="s">
+        <v>5</v>
+      </c>
       <c r="F44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I44" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Modifier","FR","Modifier");</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Modifier","EN","Edit");</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>4</v>
+      </c>
       <c r="D45" t="s">
         <v>44</v>
       </c>
+      <c r="E45" t="s">
+        <v>5</v>
+      </c>
       <c r="F45" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
-        <v>53</v>
-      </c>
-      <c r="F46" t="s">
-        <v>54</v>
+      <c r="I45" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Supprimer","FR","Supprimer");</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Supprimer","EN","Delete");</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -1165,11 +1234,11 @@
         <v>81</v>
       </c>
       <c r="I59" t="str">
-        <f t="shared" ref="I59:I66" si="0">"INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"""&amp;D59&amp;""","""&amp;C59&amp;""","""&amp;D59&amp;""");"</f>
+        <f t="shared" ref="I59:I66" si="2">"INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"""&amp;D59&amp;""","""&amp;C59&amp;""","""&amp;D59&amp;""");"</f>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Prenom","FR","Prenom");</v>
       </c>
       <c r="J59" t="str">
-        <f t="shared" ref="J59:J66" si="1">"INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"""&amp;D59&amp;""","""&amp;E59&amp;""","""&amp;F59&amp;""");"</f>
+        <f t="shared" ref="J59:J66" si="3">"INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"""&amp;D59&amp;""","""&amp;E59&amp;""","""&amp;F59&amp;""");"</f>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Prenom","EN","Last Name");</v>
       </c>
     </row>
@@ -1187,11 +1256,11 @@
         <v>82</v>
       </c>
       <c r="I60" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Mot de passe","FR","Mot de passe");</v>
       </c>
       <c r="J60" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Mot de passe","EN","Password");</v>
       </c>
     </row>
@@ -1212,11 +1281,11 @@
         <v>83</v>
       </c>
       <c r="I61" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"confirmer mot de passe","FR","confirmer mot de passe");</v>
       </c>
       <c r="J61" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"confirmer mot de passe","EN","Repeat password");</v>
       </c>
     </row>
@@ -1234,11 +1303,11 @@
         <v>77</v>
       </c>
       <c r="I62" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Age","FR","Age");</v>
       </c>
       <c r="J62" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Age","EN","Age");</v>
       </c>
     </row>
@@ -1256,11 +1325,11 @@
         <v>78</v>
       </c>
       <c r="I63" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Role","FR","Role");</v>
       </c>
       <c r="J63" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Role","EN","Role");</v>
       </c>
     </row>
@@ -1278,11 +1347,11 @@
         <v>84</v>
       </c>
       <c r="I64" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Pseudo","FR","Pseudo");</v>
       </c>
       <c r="J64" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Pseudo","EN","Nikname");</v>
       </c>
     </row>
@@ -1300,11 +1369,11 @@
         <v>87</v>
       </c>
       <c r="I65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Inscrire","FR","Inscrire");</v>
       </c>
       <c r="J65" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Inscrire","EN","Register");</v>
       </c>
     </row>
@@ -1322,17 +1391,81 @@
         <v>54</v>
       </c>
       <c r="I66" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Retour","FR","Retour");</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Retour","EN","Go back");</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
+      </c>
+      <c r="C70" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" t="s">
+        <v>89</v>
+      </c>
+      <c r="E70" t="s">
+        <v>5</v>
+      </c>
+      <c r="F70" t="s">
+        <v>90</v>
+      </c>
+      <c r="I70" t="str">
+        <f t="shared" ref="I70:I72" si="4">"INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"""&amp;D70&amp;""","""&amp;C70&amp;""","""&amp;D70&amp;""");"</f>
+        <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Ajouter une Commande","FR","Ajouter une Commande");</v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" ref="J70:J72" si="5">"INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"""&amp;D70&amp;""","""&amp;E70&amp;""","""&amp;F70&amp;""");"</f>
+        <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Ajouter une Commande","EN","Add an Order");</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" t="s">
+        <v>91</v>
+      </c>
+      <c r="E71" t="s">
+        <v>5</v>
+      </c>
+      <c r="F71" t="s">
+        <v>93</v>
+      </c>
+      <c r="I71" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Date de Commande","FR","Date de Commande");</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Date de Commande","EN","Date of Order");</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72" t="s">
+        <v>92</v>
+      </c>
+      <c r="E72" t="s">
+        <v>5</v>
+      </c>
+      <c r="F72" t="s">
+        <v>94</v>
+      </c>
+      <c r="I72" t="str">
+        <f t="shared" si="4"/>
+        <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Date de reception","FR","Date de reception");</v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" si="5"/>
+        <v>INSERT INTO Texte(idTexte, codeTexte, codeLangue, Texte) VALUES(NULL,"Date de reception","EN","Reception Date");</v>
       </c>
     </row>
   </sheetData>

</xml_diff>